<commit_message>
Improved basic UI creation
Creating Button, Image and Text are now generic
</commit_message>
<xml_diff>
--- a/RG_MaterialMod/NormalMapGreenCalculation.xlsx
+++ b/RG_MaterialMod/NormalMapGreenCalculation.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\SpockPlugins_Illusion\RG_MaterialMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A7AD81-B082-4C13-8B33-7825EB181F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897DD4C7-8766-4660-A2E3-302A096C59DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DED37834-B440-4364-B121-8ABCCE668916}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DED37834-B440-4364-B121-8ABCCE668916}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t xml:space="preserve">pink map dumped from Chara Maker </t>
   </si>
@@ -210,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -219,35 +219,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -260,6 +239,24 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -801,7 +798,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10830397924397381"/>
+          <c:y val="0.29090615104830958"/>
+          <c:w val="0.82658484930762965"/>
+          <c:h val="0.63500757414210018"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -841,11 +848,17 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.7665912450598854E-2"/>
+                  <c:y val="-0.21106584172557666"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -1218,6 +1231,421 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.35325087489063867"/>
+                  <c:y val="8.8425925925925929E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Planilha2!$S$2:$AE$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>3.1372549019607843E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10980392156862745</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.20784313725490197</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25490196078431371</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28627450980392155</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.34901960784313724</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.44313725490196076</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.50196078431372548</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.52549019607843139</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.58823529411764708</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.71372549019607845</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.792156862745098</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Planilha2!$S$3:$AE$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.19607843137254902</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36470588235294116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.49019607843137253</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54117647058823526</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5725490196078431</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.62745098039215685</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69803921568627447</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.73725490196078436</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.75294117647058822</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.792156862745098</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.83529411764705885</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.86274509803921573</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.90588235294117647</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7ECE-4B93-A12B-8DE7746345AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1719925872"/>
+        <c:axId val="1564226912"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1719925872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1564226912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1564226912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1719925872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1238,39 +1666,51 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Planilha2!$F$5:$F$14</c:f>
+              <c:f>Planilha2!$B$19:$O$19</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.99500416527802582</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98006657784124163</c:v>
+                  <c:v>-13.84988259837494</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95533648912560598</c:v>
+                  <c:v>-12.387067692545287</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9210609940028851</c:v>
+                  <c:v>-11.029924213704163</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.87758256189037276</c:v>
+                  <c:v>-9.6010513418563903</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.82533561490967833</c:v>
+                  <c:v>-8.6155794251444888</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7648421872844885</c:v>
+                  <c:v>-7.3709614534275261</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69670670934716539</c:v>
+                  <c:v>-6.1431150712228941</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.62160996827066439</c:v>
+                  <c:v>-5.5566496482017556</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.54030230586813977</c:v>
+                  <c:v>-5.1360396624084785</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-4.2341646336771248</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-3.822165106384432</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-2.8192271044040069</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.3082621935790257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1278,7 +1718,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8D2D-460E-9637-2B59EB798CEC}"/>
+              <c16:uniqueId val="{00000000-E3F6-4F56-9FFA-F3365A8AB1AD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1291,11 +1731,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2114695536"/>
-        <c:axId val="2115423648"/>
+        <c:axId val="1815662048"/>
+        <c:axId val="1566685312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2114695536"/>
+        <c:axId val="1815662048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1337,7 +1777,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115423648"/>
+        <c:crossAx val="1566685312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1345,7 +1785,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115423648"/>
+        <c:axId val="1566685312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1365,7 +1805,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1396,7 +1836,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2114695536"/>
+        <c:crossAx val="1815662048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1572,6 +2012,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2605,6 +3085,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3168,8 +4164,8 @@
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3201,23 +4197,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C0FCE36-C528-6415-4B5F-97A887DC6247}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA151D10-62C3-8A5B-08E7-D207E2E0C0DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3230,6 +4226,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>195262</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45A44177-969A-FF56-2159-79C386361230}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3537,8 +4569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91B6FCF-FFE5-4477-808B-95B2E559B1A1}">
   <dimension ref="A1:AE29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:C21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6:AE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3547,551 +4579,551 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="28"/>
-      <c r="R1" s="18" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="19"/>
+      <c r="R1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="28"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="19"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2">
         <v>50</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2">
         <v>93</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2">
         <v>125</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2">
         <v>138</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2">
         <v>146</v>
       </c>
-      <c r="H2" s="21">
+      <c r="H2">
         <v>160</v>
       </c>
-      <c r="I2" s="21">
+      <c r="I2">
         <v>178</v>
       </c>
-      <c r="J2" s="21">
+      <c r="J2">
         <v>188</v>
       </c>
-      <c r="K2" s="21">
+      <c r="K2">
         <v>192</v>
       </c>
-      <c r="L2" s="21">
+      <c r="L2">
         <v>202</v>
       </c>
-      <c r="M2" s="21">
+      <c r="M2">
         <v>213</v>
       </c>
-      <c r="N2" s="21">
+      <c r="N2">
         <v>220</v>
       </c>
-      <c r="O2" s="29">
+      <c r="O2" s="20">
         <v>231</v>
       </c>
-      <c r="R2" s="31">
-        <f>B2/255</f>
+      <c r="R2" s="22">
+        <f t="shared" ref="R2:AE2" si="0">B2/255</f>
         <v>0</v>
       </c>
-      <c r="S2" s="12">
-        <f>C2/255</f>
+      <c r="S2" s="3">
+        <f t="shared" si="0"/>
         <v>0.19607843137254902</v>
       </c>
-      <c r="T2" s="12">
-        <f>D2/255</f>
+      <c r="T2" s="3">
+        <f t="shared" si="0"/>
         <v>0.36470588235294116</v>
       </c>
-      <c r="U2" s="12">
-        <f>E2/255</f>
+      <c r="U2" s="3">
+        <f t="shared" si="0"/>
         <v>0.49019607843137253</v>
       </c>
-      <c r="V2" s="12">
-        <f>F2/255</f>
+      <c r="V2" s="3">
+        <f t="shared" si="0"/>
         <v>0.54117647058823526</v>
       </c>
-      <c r="W2" s="12">
-        <f>G2/255</f>
+      <c r="W2" s="3">
+        <f t="shared" si="0"/>
         <v>0.5725490196078431</v>
       </c>
-      <c r="X2" s="12">
-        <f>H2/255</f>
+      <c r="X2" s="3">
+        <f t="shared" si="0"/>
         <v>0.62745098039215685</v>
       </c>
-      <c r="Y2" s="12">
-        <f>I2/255</f>
+      <c r="Y2" s="3">
+        <f t="shared" si="0"/>
         <v>0.69803921568627447</v>
       </c>
-      <c r="Z2" s="12">
-        <f>J2/255</f>
+      <c r="Z2" s="3">
+        <f t="shared" si="0"/>
         <v>0.73725490196078436</v>
       </c>
-      <c r="AA2" s="12">
-        <f>K2/255</f>
+      <c r="AA2" s="3">
+        <f t="shared" si="0"/>
         <v>0.75294117647058822</v>
       </c>
-      <c r="AB2" s="12">
-        <f>L2/255</f>
+      <c r="AB2" s="3">
+        <f t="shared" si="0"/>
         <v>0.792156862745098</v>
       </c>
-      <c r="AC2" s="12">
-        <f>M2/255</f>
+      <c r="AC2" s="3">
+        <f t="shared" si="0"/>
         <v>0.83529411764705885</v>
       </c>
-      <c r="AD2" s="12">
-        <f>N2/255</f>
+      <c r="AD2" s="3">
+        <f t="shared" si="0"/>
         <v>0.86274509803921573</v>
       </c>
-      <c r="AE2" s="13">
-        <f>O2/255</f>
+      <c r="AE2" s="8">
+        <f t="shared" si="0"/>
         <v>0.90588235294117647</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="16">
         <v>127</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="16">
         <v>127</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="16">
         <v>130</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="16">
         <v>121</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="16">
         <v>168</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="16">
         <v>116</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="16">
         <v>126</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="16">
         <v>72</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="16">
         <v>128</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3" s="16">
         <v>118</v>
       </c>
-      <c r="L3" s="25">
+      <c r="L3" s="16">
         <v>58</v>
       </c>
-      <c r="M3" s="25">
+      <c r="M3" s="16">
         <v>90</v>
       </c>
-      <c r="N3" s="25">
+      <c r="N3" s="16">
         <v>179</v>
       </c>
-      <c r="O3" s="30">
+      <c r="O3" s="21">
         <v>102</v>
       </c>
-      <c r="R3" s="32">
-        <f>B6/255</f>
+      <c r="R3" s="23">
+        <f t="shared" ref="R3:AE3" si="1">B6/255</f>
         <v>0</v>
       </c>
-      <c r="S3" s="16">
-        <f>C6/255</f>
+      <c r="S3" s="9">
+        <f t="shared" si="1"/>
         <v>3.1372549019607843E-2</v>
       </c>
-      <c r="T3" s="16">
-        <f>D6/255</f>
+      <c r="T3" s="9">
+        <f t="shared" si="1"/>
         <v>0.10980392156862745</v>
       </c>
-      <c r="U3" s="16">
-        <f>E6/255</f>
+      <c r="U3" s="9">
+        <f t="shared" si="1"/>
         <v>0.20784313725490197</v>
       </c>
-      <c r="V3" s="16">
-        <f>F6/255</f>
+      <c r="V3" s="9">
+        <f t="shared" si="1"/>
         <v>0.25490196078431371</v>
       </c>
-      <c r="W3" s="16">
-        <f>G6/255</f>
+      <c r="W3" s="9">
+        <f t="shared" si="1"/>
         <v>0.28627450980392155</v>
       </c>
-      <c r="X3" s="16">
-        <f>H6/255</f>
+      <c r="X3" s="9">
+        <f t="shared" si="1"/>
         <v>0.34901960784313724</v>
       </c>
-      <c r="Y3" s="16">
-        <f>I6/255</f>
+      <c r="Y3" s="9">
+        <f t="shared" si="1"/>
         <v>0.44313725490196076</v>
       </c>
-      <c r="Z3" s="16">
-        <f>J6/255</f>
+      <c r="Z3" s="9">
+        <f t="shared" si="1"/>
         <v>0.50196078431372548</v>
       </c>
-      <c r="AA3" s="16">
-        <f>K6/255</f>
+      <c r="AA3" s="9">
+        <f t="shared" si="1"/>
         <v>0.52549019607843139</v>
       </c>
-      <c r="AB3" s="16">
-        <f>L6/255</f>
+      <c r="AB3" s="9">
+        <f t="shared" si="1"/>
         <v>0.58823529411764708</v>
       </c>
-      <c r="AC3" s="16">
-        <f>M6/255</f>
+      <c r="AC3" s="9">
+        <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="AD3" s="16">
-        <f>N6/255</f>
+      <c r="AD3" s="9">
+        <f t="shared" si="1"/>
         <v>0.71372549019607845</v>
       </c>
-      <c r="AE3" s="17">
-        <f>O6/255</f>
+      <c r="AE3" s="10">
+        <f t="shared" si="1"/>
         <v>0.792156862745098</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="28"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="19" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="19"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="19"/>
-      <c r="X5" s="19"/>
-      <c r="Y5" s="19"/>
-      <c r="Z5" s="19"/>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="19"/>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="19"/>
-      <c r="AE5" s="28"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="12"/>
+      <c r="AE5" s="19"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6">
         <v>8</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6">
         <v>28</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6">
         <v>53</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6">
         <v>65</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6">
         <v>73</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6">
         <v>89</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6">
         <v>113</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6">
         <v>128</v>
       </c>
-      <c r="K6" s="21">
+      <c r="K6">
         <v>134</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6">
         <v>150</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6">
         <v>170</v>
       </c>
-      <c r="N6" s="21">
+      <c r="N6">
         <v>182</v>
       </c>
-      <c r="O6" s="29">
+      <c r="O6" s="20">
         <v>202</v>
       </c>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="21">
-        <f t="shared" ref="R6:AE6" si="0">1.1049*R2^2-0.1386*R2+0.007</f>
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="S6" s="21">
-        <f t="shared" si="0"/>
-        <v>2.2303344867358701E-2</v>
-      </c>
-      <c r="T6" s="21">
-        <f t="shared" si="0"/>
-        <v>0.10341493425605536</v>
-      </c>
-      <c r="U6" s="21">
-        <f t="shared" si="0"/>
-        <v>0.20455767012687426</v>
-      </c>
-      <c r="V6" s="21">
-        <f t="shared" si="0"/>
-        <v>0.25558718339100339</v>
-      </c>
-      <c r="W6" s="21">
-        <f t="shared" si="0"/>
-        <v>0.28984460438292958</v>
-      </c>
-      <c r="X6" s="21">
-        <f t="shared" si="0"/>
-        <v>0.35502860438292966</v>
-      </c>
-      <c r="Y6" s="21">
-        <f t="shared" si="0"/>
-        <v>0.44862395386389847</v>
-      </c>
-      <c r="Z6" s="21">
-        <f t="shared" si="0"/>
-        <v>0.50537910957324106</v>
-      </c>
-      <c r="AA6" s="21">
-        <f t="shared" si="0"/>
-        <v>0.52903271972318333</v>
-      </c>
-      <c r="AB6" s="21">
-        <f t="shared" si="0"/>
-        <v>0.5905456147635525</v>
-      </c>
-      <c r="AC6" s="21">
-        <f t="shared" si="0"/>
-        <v>0.66213493425605541</v>
-      </c>
-      <c r="AD6" s="21">
-        <f t="shared" si="0"/>
-        <v>0.70983275663206469</v>
-      </c>
-      <c r="AE6" s="29">
-        <f t="shared" si="0"/>
-        <v>0.7881508788927335</v>
+      <c r="Q6" s="13"/>
+      <c r="R6">
+        <f>0.294115*R2^3 +0.69229*R2^2 +0.009424*R2+0.000233</f>
+        <v>2.33E-4</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ref="S6:AE6" si="2">0.294115*S2^3 +0.69229*S2^2 +0.009424*S2+0.000233</f>
+        <v>3.0914353627187131E-2</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="2"/>
+        <v>0.11001916570730712</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="2"/>
+        <v>0.20584838341211145</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="2"/>
+        <v>0.25470126532057802</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="2"/>
+        <v>0.28777198367535861</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="2"/>
+        <v>0.35135053132656369</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="2"/>
+        <v>0.44417175345560905</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="2"/>
+        <v>0.50133252925375615</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="2"/>
+        <v>0.52534731151638514</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="2"/>
+        <v>0.58832004561111484</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" si="2"/>
+        <v>0.6625365225971912</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="2"/>
+        <v>0.71252584254170737</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" si="2"/>
+        <v>0.79552050652554451</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="16">
         <v>127</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="16">
         <v>127</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="16">
         <v>130</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="16">
         <v>121</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="16">
         <v>168</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="16">
         <v>116</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="16">
         <v>126</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="16">
         <v>72</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="16">
         <v>128</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="16">
         <v>118</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="16">
         <v>58</v>
       </c>
-      <c r="M7" s="25">
+      <c r="M7" s="16">
         <v>90</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="16">
         <v>179</v>
       </c>
-      <c r="O7" s="30">
+      <c r="O7" s="21">
         <v>102</v>
       </c>
-      <c r="Q7" s="20" t="s">
+      <c r="Q7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="22">
+      <c r="R7" s="4">
         <f>R6*255</f>
-        <v>1.7850000000000001</v>
-      </c>
-      <c r="S7" s="22">
+        <v>5.9415000000000003E-2</v>
+      </c>
+      <c r="S7" s="4">
         <f>S6*255</f>
-        <v>5.6873529411764689</v>
-      </c>
-      <c r="T7" s="22">
-        <f t="shared" ref="T7:AE7" si="1">T6*255</f>
-        <v>26.370808235294117</v>
-      </c>
-      <c r="U7" s="22">
-        <f t="shared" si="1"/>
-        <v>52.162205882352936</v>
-      </c>
-      <c r="V7" s="22">
-        <f t="shared" si="1"/>
-        <v>65.174731764705868</v>
-      </c>
-      <c r="W7" s="22">
-        <f t="shared" si="1"/>
-        <v>73.910374117647038</v>
-      </c>
-      <c r="X7" s="22">
-        <f t="shared" si="1"/>
-        <v>90.532294117647069</v>
-      </c>
-      <c r="Y7" s="22">
-        <f t="shared" si="1"/>
-        <v>114.39910823529411</v>
-      </c>
-      <c r="Z7" s="22">
-        <f t="shared" si="1"/>
-        <v>128.87167294117646</v>
-      </c>
-      <c r="AA7" s="22">
-        <f t="shared" si="1"/>
-        <v>134.90334352941176</v>
-      </c>
-      <c r="AB7" s="22">
-        <f t="shared" si="1"/>
-        <v>150.58913176470588</v>
-      </c>
-      <c r="AC7" s="22">
-        <f t="shared" si="1"/>
-        <v>168.84440823529414</v>
-      </c>
-      <c r="AD7" s="22">
-        <f t="shared" si="1"/>
-        <v>181.00735294117649</v>
-      </c>
-      <c r="AE7" s="23">
-        <f t="shared" si="1"/>
-        <v>200.97847411764704</v>
+        <v>7.8831601749327183</v>
+      </c>
+      <c r="T7" s="4">
+        <f t="shared" ref="T7:AE7" si="3">T6*255</f>
+        <v>28.054887255363315</v>
+      </c>
+      <c r="U7" s="4">
+        <f t="shared" si="3"/>
+        <v>52.491337770088421</v>
+      </c>
+      <c r="V7" s="4">
+        <f t="shared" si="3"/>
+        <v>64.948822656747396</v>
+      </c>
+      <c r="W7" s="4">
+        <f t="shared" si="3"/>
+        <v>73.381855837216449</v>
+      </c>
+      <c r="X7" s="4">
+        <f t="shared" si="3"/>
+        <v>89.594385488273744</v>
+      </c>
+      <c r="Y7" s="4">
+        <f t="shared" si="3"/>
+        <v>113.26379713118031</v>
+      </c>
+      <c r="Z7" s="4">
+        <f t="shared" si="3"/>
+        <v>127.83979495970782</v>
+      </c>
+      <c r="AA7" s="4">
+        <f t="shared" si="3"/>
+        <v>133.96356443667821</v>
+      </c>
+      <c r="AB7" s="4">
+        <f t="shared" si="3"/>
+        <v>150.02161163083429</v>
+      </c>
+      <c r="AC7" s="4">
+        <f t="shared" si="3"/>
+        <v>168.94681326228377</v>
+      </c>
+      <c r="AD7" s="4">
+        <f t="shared" si="3"/>
+        <v>181.69408984813538</v>
+      </c>
+      <c r="AE7" s="14">
+        <f t="shared" si="3"/>
+        <v>202.85772916401385</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="Q8" s="24" t="s">
+      <c r="Q8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="26">
-        <f>R7-B6</f>
-        <v>1.7850000000000001</v>
-      </c>
-      <c r="S8" s="26">
-        <f>S7-C6</f>
-        <v>-2.3126470588235311</v>
-      </c>
-      <c r="T8" s="26">
-        <f>T7-D6</f>
-        <v>-1.6291917647058831</v>
-      </c>
-      <c r="U8" s="26">
-        <f>U7-E6</f>
-        <v>-0.83779411764706424</v>
-      </c>
-      <c r="V8" s="26">
-        <f>V7-F6</f>
-        <v>0.17473176470586793</v>
-      </c>
-      <c r="W8" s="26">
-        <f>W7-G6</f>
-        <v>0.91037411764703791</v>
-      </c>
-      <c r="X8" s="26">
-        <f>X7-H6</f>
-        <v>1.5322941176470692</v>
-      </c>
-      <c r="Y8" s="26">
-        <f>Y7-I6</f>
-        <v>1.3991082352941078</v>
-      </c>
-      <c r="Z8" s="26">
-        <f>Z7-J6</f>
-        <v>0.87167294117645611</v>
-      </c>
-      <c r="AA8" s="26">
-        <f>AA7-K6</f>
-        <v>0.90334352941175666</v>
-      </c>
-      <c r="AB8" s="26">
-        <f>AB7-L6</f>
-        <v>0.58913176470588269</v>
-      </c>
-      <c r="AC8" s="26">
-        <f>AC7-M6</f>
-        <v>-1.1555917647058607</v>
-      </c>
-      <c r="AD8" s="26">
-        <f>AD7-N6</f>
-        <v>-0.99264705882350768</v>
-      </c>
-      <c r="AE8" s="27">
-        <f>AE7-O6</f>
-        <v>-1.0215258823529609</v>
+      <c r="R8" s="17">
+        <f t="shared" ref="R8:AE8" si="4">R7-B6</f>
+        <v>5.9415000000000003E-2</v>
+      </c>
+      <c r="S8" s="17">
+        <f t="shared" si="4"/>
+        <v>-0.11683982506728174</v>
+      </c>
+      <c r="T8" s="17">
+        <f t="shared" si="4"/>
+        <v>5.488725536331529E-2</v>
+      </c>
+      <c r="U8" s="17">
+        <f t="shared" si="4"/>
+        <v>-0.50866222991157883</v>
+      </c>
+      <c r="V8" s="17">
+        <f t="shared" si="4"/>
+        <v>-5.1177343252604146E-2</v>
+      </c>
+      <c r="W8" s="17">
+        <f t="shared" si="4"/>
+        <v>0.38185583721644889</v>
+      </c>
+      <c r="X8" s="17">
+        <f t="shared" si="4"/>
+        <v>0.59438548827374404</v>
+      </c>
+      <c r="Y8" s="17">
+        <f t="shared" si="4"/>
+        <v>0.26379713118031134</v>
+      </c>
+      <c r="Z8" s="17">
+        <f t="shared" si="4"/>
+        <v>-0.1602050402921833</v>
+      </c>
+      <c r="AA8" s="17">
+        <f t="shared" si="4"/>
+        <v>-3.6435563321788322E-2</v>
+      </c>
+      <c r="AB8" s="17">
+        <f t="shared" si="4"/>
+        <v>2.1611630834286188E-2</v>
+      </c>
+      <c r="AC8" s="17">
+        <f t="shared" si="4"/>
+        <v>-1.0531867377162314</v>
+      </c>
+      <c r="AD8" s="17">
+        <f t="shared" si="4"/>
+        <v>-0.305910151864623</v>
+      </c>
+      <c r="AE8" s="18">
+        <f t="shared" si="4"/>
+        <v>0.85772916401384691</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -4152,173 +5184,173 @@
       <c r="M16" s="2"/>
     </row>
     <row r="17" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="24" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="8">
-        <f>B2/255</f>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="6">
+        <f t="shared" ref="D18:Q18" si="5">B2/255</f>
         <v>0</v>
       </c>
-      <c r="E18" s="8">
-        <f>C2/255</f>
+      <c r="E18" s="6">
+        <f t="shared" si="5"/>
         <v>0.19607843137254902</v>
       </c>
-      <c r="F18" s="8">
-        <f>D2/255</f>
+      <c r="F18" s="6">
+        <f t="shared" si="5"/>
         <v>0.36470588235294116</v>
       </c>
-      <c r="G18" s="8">
-        <f>E2/255</f>
+      <c r="G18" s="6">
+        <f t="shared" si="5"/>
         <v>0.49019607843137253</v>
       </c>
-      <c r="H18" s="8">
-        <f>F2/255</f>
+      <c r="H18" s="6">
+        <f t="shared" si="5"/>
         <v>0.54117647058823526</v>
       </c>
-      <c r="I18" s="8">
-        <f>G2/255</f>
+      <c r="I18" s="6">
+        <f t="shared" si="5"/>
         <v>0.5725490196078431</v>
       </c>
-      <c r="J18" s="8">
-        <f>H2/255</f>
+      <c r="J18" s="6">
+        <f t="shared" si="5"/>
         <v>0.62745098039215685</v>
       </c>
-      <c r="K18" s="8">
-        <f>I2/255</f>
+      <c r="K18" s="6">
+        <f t="shared" si="5"/>
         <v>0.69803921568627447</v>
       </c>
-      <c r="L18" s="8">
-        <f>J2/255</f>
+      <c r="L18" s="6">
+        <f t="shared" si="5"/>
         <v>0.73725490196078436</v>
       </c>
-      <c r="M18" s="8">
-        <f>K2/255</f>
+      <c r="M18" s="6">
+        <f t="shared" si="5"/>
         <v>0.75294117647058822</v>
       </c>
-      <c r="N18" s="8">
-        <f>L2/255</f>
+      <c r="N18" s="6">
+        <f t="shared" si="5"/>
         <v>0.792156862745098</v>
       </c>
-      <c r="O18" s="8">
-        <f>M2/255</f>
+      <c r="O18" s="6">
+        <f t="shared" si="5"/>
         <v>0.83529411764705885</v>
       </c>
-      <c r="P18" s="8">
-        <f>N2/255</f>
+      <c r="P18" s="6">
+        <f t="shared" si="5"/>
         <v>0.86274509803921573</v>
       </c>
-      <c r="Q18" s="9">
-        <f>O2/255</f>
+      <c r="Q18" s="7">
+        <f t="shared" si="5"/>
         <v>0.90588235294117647</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="28"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="19"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12">
-        <f>D18-SQRT(R3)</f>
+      <c r="A20" s="27"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="3">
+        <f t="shared" ref="D20:Q20" si="6">D18-SQRT(R3)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="12">
-        <f>E18-SQRT(S3)</f>
+      <c r="E20" s="3">
+        <f t="shared" si="6"/>
         <v>1.8955454264529964E-2</v>
       </c>
-      <c r="F20" s="12">
-        <f>F18-SQRT(T3)</f>
+      <c r="F20" s="3">
+        <f t="shared" si="6"/>
         <v>3.3339134521135572E-2</v>
       </c>
-      <c r="G20" s="12">
-        <f>G18-SQRT(U3)</f>
+      <c r="G20" s="3">
+        <f t="shared" si="6"/>
         <v>3.4297912987704626E-2</v>
       </c>
-      <c r="H20" s="12">
-        <f>H18-SQRT(V3)</f>
+      <c r="H20" s="3">
+        <f t="shared" si="6"/>
         <v>3.629830629083397E-2</v>
       </c>
-      <c r="I20" s="12">
-        <f>I18-SQRT(W3)</f>
+      <c r="I20" s="3">
+        <f t="shared" si="6"/>
         <v>3.7502750763809822E-2</v>
       </c>
-      <c r="J20" s="12">
-        <f>J18-SQRT(X3)</f>
+      <c r="J20" s="3">
+        <f t="shared" si="6"/>
         <v>3.6672165738874551E-2</v>
       </c>
-      <c r="K20" s="12">
-        <f>K18-SQRT(Y3)</f>
+      <c r="K20" s="3">
+        <f t="shared" si="6"/>
         <v>3.2353663115121889E-2</v>
       </c>
-      <c r="L20" s="12">
-        <f>L18-SQRT(Z3)</f>
+      <c r="L20" s="3">
+        <f t="shared" si="6"/>
         <v>2.8762993528708147E-2</v>
       </c>
-      <c r="M20" s="12">
-        <f>M18-SQRT(AA3)</f>
+      <c r="M20" s="3">
+        <f t="shared" si="6"/>
         <v>2.8034150653876044E-2</v>
       </c>
-      <c r="N20" s="12">
-        <f>N18-SQRT(AB3)</f>
+      <c r="N20" s="3">
+        <f t="shared" si="6"/>
         <v>2.519187389772759E-2</v>
       </c>
-      <c r="O20" s="12">
-        <f>O18-SQRT(AC3)</f>
+      <c r="O20" s="3">
+        <f t="shared" si="6"/>
         <v>1.8797536719332819E-2</v>
       </c>
-      <c r="P20" s="12">
-        <f>P18-SQRT(AD3)</f>
+      <c r="P20" s="3">
+        <f t="shared" si="6"/>
         <v>1.7922341364137506E-2</v>
       </c>
-      <c r="Q20" s="13">
-        <f>Q18-SQRT(AE3)</f>
+      <c r="Q20" s="8">
+        <f t="shared" si="6"/>
         <v>1.5850408152059403E-2</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="17"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="10"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D22" s="3"/>
@@ -4337,105 +5369,105 @@
       <c r="Q22" s="3"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="9"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="7"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12">
-        <f>-0.142436*R2^2+0.146477*R2 -0.001472</f>
+      <c r="A24" s="27"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="3">
+        <f t="shared" ref="D24:Q24" si="7">-0.142436*R2^2+0.146477*R2 -0.001472</f>
         <v>-1.472E-3</v>
       </c>
-      <c r="E24" s="12">
-        <f>-0.142436*S2^2+0.146477*S2 -0.001472</f>
+      <c r="E24" s="3">
+        <f t="shared" si="7"/>
         <v>2.1772778931180313E-2</v>
       </c>
-      <c r="F24" s="12">
-        <f>-0.142436*T2^2+0.146477*T2 -0.001472</f>
+      <c r="F24" s="3">
+        <f t="shared" si="7"/>
         <v>3.3003556955017305E-2</v>
       </c>
-      <c r="G24" s="12">
-        <f>-0.142436*U2^2+0.146477*U2 -0.001472</f>
+      <c r="G24" s="3">
+        <f t="shared" si="7"/>
         <v>3.6104191849288723E-2</v>
       </c>
-      <c r="H24" s="12">
-        <f>-0.142436*V2^2+0.146477*V2 -0.001472</f>
+      <c r="H24" s="3">
+        <f t="shared" si="7"/>
         <v>3.6082393633217982E-2</v>
       </c>
-      <c r="I24" s="12">
-        <f>-0.142436*W2^2+0.146477*W2 -0.001472</f>
+      <c r="I24" s="3">
+        <f t="shared" si="7"/>
         <v>3.5700978608227601E-2</v>
       </c>
-      <c r="J24" s="12">
-        <f>-0.142436*X2^2+0.146477*X2 -0.001472</f>
+      <c r="J24" s="3">
+        <f t="shared" si="7"/>
         <v>3.4358834294502108E-2</v>
       </c>
-      <c r="K24" s="12">
-        <f>-0.142436*Y2^2+0.146477*Y2 -0.001472</f>
+      <c r="K24" s="3">
+        <f t="shared" si="7"/>
         <v>3.137150336024605E-2</v>
       </c>
-      <c r="L24" s="12">
-        <f>-0.142436*Z2^2+0.146477*Z2 -0.001472</f>
+      <c r="L24" s="3">
+        <f t="shared" si="7"/>
         <v>2.9098540499807757E-2</v>
       </c>
-      <c r="M24" s="12">
-        <f>-0.142436*AA2^2+0.146477*AA2 -0.001472</f>
+      <c r="M24" s="3">
+        <f t="shared" si="7"/>
         <v>2.8066688442906565E-2</v>
       </c>
-      <c r="N24" s="12">
-        <f>-0.142436*AB2^2+0.146477*AB2 -0.001472</f>
+      <c r="N24" s="3">
+        <f t="shared" si="7"/>
         <v>2.5180391018838885E-2</v>
       </c>
-      <c r="O24" s="12">
-        <f>-0.142436*AC2^2+0.146477*AC2 -0.001472</f>
+      <c r="O24" s="3">
+        <f t="shared" si="7"/>
         <v>2.1499462837370226E-2</v>
       </c>
-      <c r="P24" s="12">
-        <f>-0.142436*AD2^2+0.146477*AD2 -0.001472</f>
+      <c r="P24" s="3">
+        <f t="shared" si="7"/>
         <v>1.888105344098423E-2</v>
       </c>
-      <c r="Q24" s="13">
-        <f>-0.142436*AE2^2+0.146477*AE2 -0.001472</f>
+      <c r="Q24" s="8">
+        <f t="shared" si="7"/>
         <v>1.433269494809686E-2</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="17"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="10"/>
     </row>
     <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
@@ -4457,191 +5489,189 @@
       <c r="Q26" s="3"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="8">
-        <f>(R2-D24)^2</f>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="6">
+        <f t="shared" ref="D27:Q27" si="8">(R2-D24)^2</f>
         <v>2.1667840000000001E-6</v>
       </c>
-      <c r="E27" s="8">
-        <f>(S2-E24)^2</f>
+      <c r="E27" s="6">
+        <f t="shared" si="8"/>
         <v>3.038246047301122E-2</v>
       </c>
-      <c r="F27" s="8">
-        <f>(T2-F24)^2</f>
+      <c r="F27" s="6">
+        <f t="shared" si="8"/>
         <v>0.11002643267439018</v>
       </c>
-      <c r="G27" s="8">
-        <f>(U2-G24)^2</f>
+      <c r="G27" s="6">
+        <f t="shared" si="8"/>
         <v>0.20619944145967609</v>
       </c>
-      <c r="H27" s="8">
-        <f>(V2-H24)^2</f>
+      <c r="H27" s="6">
+        <f t="shared" si="8"/>
         <v>0.2551200265750409</v>
       </c>
-      <c r="I27" s="8">
-        <f>(W2-I24)^2</f>
+      <c r="I27" s="6">
+        <f t="shared" si="8"/>
         <v>0.28820581912512483</v>
       </c>
-      <c r="J27" s="8">
-        <f>(X2-J24)^2</f>
+      <c r="J27" s="6">
+        <f t="shared" si="8"/>
         <v>0.35175829376272177</v>
       </c>
-      <c r="K27" s="8">
-        <f>(Y2-K24)^2</f>
+      <c r="K27" s="6">
+        <f t="shared" si="8"/>
         <v>0.44444583865802018</v>
       </c>
-      <c r="L27" s="8">
-        <f>(Z2-L24)^2</f>
+      <c r="L27" s="6">
+        <f t="shared" si="8"/>
         <v>0.5014854322776493</v>
       </c>
-      <c r="M27" s="8">
-        <f>(AA2-M24)^2</f>
+      <c r="M27" s="6">
+        <f t="shared" si="8"/>
         <v>0.52544302339339355</v>
       </c>
-      <c r="N27" s="8">
-        <f>(AB2-N24)^2</f>
+      <c r="N27" s="6">
+        <f t="shared" si="8"/>
         <v>0.5882529081816612</v>
       </c>
-      <c r="O27" s="8">
-        <f>(AC2-O24)^2</f>
+      <c r="O27" s="6">
+        <f t="shared" si="8"/>
         <v>0.66226174019682027</v>
       </c>
-      <c r="P27" s="8">
-        <f>(AD2-P24)^2</f>
+      <c r="P27" s="6">
+        <f t="shared" si="8"/>
         <v>0.712106525765686</v>
       </c>
-      <c r="Q27" s="9">
-        <f>(AE2-Q24)^2</f>
+      <c r="Q27" s="7">
+        <f t="shared" si="8"/>
         <v>0.79486079266757725</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22">
+      <c r="D28" s="4">
         <f>D27*255</f>
         <v>5.5252992000000007E-4</v>
       </c>
-      <c r="E28" s="22">
-        <f t="shared" ref="E28:Q28" si="2">E27*255</f>
+      <c r="E28" s="4">
+        <f t="shared" ref="E28:Q28" si="9">E27*255</f>
         <v>7.7475274206178613</v>
       </c>
-      <c r="F28" s="22">
-        <f t="shared" si="2"/>
+      <c r="F28" s="4">
+        <f t="shared" si="9"/>
         <v>28.056740331969493</v>
       </c>
-      <c r="G28" s="22">
-        <f t="shared" si="2"/>
+      <c r="G28" s="4">
+        <f t="shared" si="9"/>
         <v>52.580857572217404</v>
       </c>
-      <c r="H28" s="22">
-        <f t="shared" si="2"/>
+      <c r="H28" s="4">
+        <f t="shared" si="9"/>
         <v>65.055606776635429</v>
       </c>
-      <c r="I28" s="22">
-        <f t="shared" si="2"/>
+      <c r="I28" s="4">
+        <f t="shared" si="9"/>
         <v>73.492483876906832</v>
       </c>
-      <c r="J28" s="22">
-        <f t="shared" si="2"/>
+      <c r="J28" s="4">
+        <f t="shared" si="9"/>
         <v>89.698364909494046</v>
       </c>
-      <c r="K28" s="22">
-        <f t="shared" si="2"/>
+      <c r="K28" s="4">
+        <f t="shared" si="9"/>
         <v>113.33368885779514</v>
       </c>
-      <c r="L28" s="22">
-        <f t="shared" si="2"/>
+      <c r="L28" s="4">
+        <f t="shared" si="9"/>
         <v>127.87878523080057</v>
       </c>
-      <c r="M28" s="22">
-        <f t="shared" si="2"/>
+      <c r="M28" s="4">
+        <f t="shared" si="9"/>
         <v>133.98797096531536</v>
       </c>
-      <c r="N28" s="22">
-        <f t="shared" si="2"/>
+      <c r="N28" s="4">
+        <f t="shared" si="9"/>
         <v>150.00449158632361</v>
       </c>
-      <c r="O28" s="22">
-        <f t="shared" si="2"/>
+      <c r="O28" s="4">
+        <f t="shared" si="9"/>
         <v>168.87674375018918</v>
       </c>
-      <c r="P28" s="22">
-        <f t="shared" si="2"/>
+      <c r="P28" s="4">
+        <f t="shared" si="9"/>
         <v>181.58716407024994</v>
       </c>
-      <c r="Q28" s="23">
-        <f t="shared" si="2"/>
+      <c r="Q28" s="14">
+        <f t="shared" si="9"/>
         <v>202.6895021302322</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="26">
-        <f>D28-B6</f>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17">
+        <f t="shared" ref="D29:Q29" si="10">D28-B6</f>
         <v>5.5252992000000007E-4</v>
       </c>
-      <c r="E29" s="26">
-        <f>E28-C6</f>
+      <c r="E29" s="17">
+        <f t="shared" si="10"/>
         <v>-0.25247257938213874</v>
       </c>
-      <c r="F29" s="26">
-        <f>F28-D6</f>
+      <c r="F29" s="17">
+        <f t="shared" si="10"/>
         <v>5.6740331969493241E-2</v>
       </c>
-      <c r="G29" s="26">
-        <f>G28-E6</f>
+      <c r="G29" s="17">
+        <f t="shared" si="10"/>
         <v>-0.41914242778259592</v>
       </c>
-      <c r="H29" s="26">
-        <f>H28-F6</f>
+      <c r="H29" s="17">
+        <f t="shared" si="10"/>
         <v>5.5606776635428901E-2</v>
       </c>
-      <c r="I29" s="26">
-        <f>I28-G6</f>
+      <c r="I29" s="17">
+        <f t="shared" si="10"/>
         <v>0.4924838769068316</v>
       </c>
-      <c r="J29" s="26">
-        <f>J28-H6</f>
+      <c r="J29" s="17">
+        <f t="shared" si="10"/>
         <v>0.69836490949404606</v>
       </c>
-      <c r="K29" s="26">
-        <f>K28-I6</f>
+      <c r="K29" s="17">
+        <f t="shared" si="10"/>
         <v>0.33368885779513846</v>
       </c>
-      <c r="L29" s="26">
-        <f>L28-J6</f>
+      <c r="L29" s="17">
+        <f t="shared" si="10"/>
         <v>-0.12121476919942609</v>
       </c>
-      <c r="M29" s="26">
-        <f>M28-K6</f>
+      <c r="M29" s="17">
+        <f t="shared" si="10"/>
         <v>-1.2029034684644557E-2</v>
       </c>
-      <c r="N29" s="26">
-        <f>N28-L6</f>
+      <c r="N29" s="17">
+        <f t="shared" si="10"/>
         <v>4.4915863236099085E-3</v>
       </c>
-      <c r="O29" s="26">
-        <f>O28-M6</f>
+      <c r="O29" s="17">
+        <f t="shared" si="10"/>
         <v>-1.1232562498108223</v>
       </c>
-      <c r="P29" s="26">
-        <f>P28-N6</f>
+      <c r="P29" s="17">
+        <f t="shared" si="10"/>
         <v>-0.41283592975005945</v>
       </c>
-      <c r="Q29" s="27">
-        <f>Q28-O6</f>
+      <c r="Q29" s="18">
+        <f t="shared" si="10"/>
         <v>0.68950213023219931</v>
       </c>
     </row>
@@ -4657,104 +5687,867 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5845AC-C4A5-473C-A4F6-FA7D4998A0B4}">
-  <dimension ref="C5:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7562675D-190A-4CFA-870E-5F669E849159}">
+  <dimension ref="A1:AE22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5:AE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="52" width="6" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>0.1</v>
-      </c>
-      <c r="F5">
-        <f>COS(C5)</f>
-        <v>0.99500416527802582</v>
-      </c>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="19"/>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>93</v>
+      </c>
+      <c r="E2">
+        <v>125</v>
+      </c>
+      <c r="F2">
+        <v>138</v>
+      </c>
+      <c r="G2">
+        <v>146</v>
+      </c>
+      <c r="H2">
+        <v>160</v>
+      </c>
+      <c r="I2">
+        <v>178</v>
+      </c>
+      <c r="J2">
+        <v>188</v>
+      </c>
+      <c r="K2">
+        <v>192</v>
+      </c>
+      <c r="L2">
+        <v>202</v>
+      </c>
+      <c r="M2">
+        <v>213</v>
+      </c>
+      <c r="N2">
+        <v>220</v>
+      </c>
+      <c r="O2" s="20">
+        <v>231</v>
+      </c>
+      <c r="R2" s="3">
+        <f>B6/255</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="3">
+        <f t="shared" ref="S2:AE2" si="0">C6/255</f>
+        <v>3.1372549019607843E-2</v>
+      </c>
+      <c r="T2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.10980392156862745</v>
+      </c>
+      <c r="U2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.20784313725490197</v>
+      </c>
+      <c r="V2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.25490196078431371</v>
+      </c>
+      <c r="W2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.28627450980392155</v>
+      </c>
+      <c r="X2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.34901960784313724</v>
+      </c>
+      <c r="Y2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.44313725490196076</v>
+      </c>
+      <c r="Z2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.50196078431372548</v>
+      </c>
+      <c r="AA2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.52549019607843139</v>
+      </c>
+      <c r="AB2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="AC2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AD2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.71372549019607845</v>
+      </c>
+      <c r="AE2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.792156862745098</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="16">
+        <v>127</v>
+      </c>
+      <c r="C3" s="16">
+        <v>127</v>
+      </c>
+      <c r="D3" s="16">
+        <v>130</v>
+      </c>
+      <c r="E3" s="16">
+        <v>121</v>
+      </c>
+      <c r="F3" s="16">
+        <v>168</v>
+      </c>
+      <c r="G3" s="16">
+        <v>116</v>
+      </c>
+      <c r="H3" s="16">
+        <v>126</v>
+      </c>
+      <c r="I3" s="16">
+        <v>72</v>
+      </c>
+      <c r="J3" s="16">
+        <v>128</v>
+      </c>
+      <c r="K3" s="16">
+        <v>118</v>
+      </c>
+      <c r="L3" s="16">
+        <v>58</v>
+      </c>
+      <c r="M3" s="16">
+        <v>90</v>
+      </c>
+      <c r="N3" s="16">
+        <v>179</v>
+      </c>
+      <c r="O3" s="21">
+        <v>102</v>
+      </c>
+      <c r="R3" s="3">
+        <f>B2/255</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="3">
+        <f t="shared" ref="S3:AE3" si="1">C2/255</f>
+        <v>0.19607843137254902</v>
+      </c>
+      <c r="T3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.36470588235294116</v>
+      </c>
+      <c r="U3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.49019607843137253</v>
+      </c>
+      <c r="V3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.54117647058823526</v>
+      </c>
+      <c r="W3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.5725490196078431</v>
+      </c>
+      <c r="X3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.62745098039215685</v>
+      </c>
+      <c r="Y3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.69803921568627447</v>
+      </c>
+      <c r="Z3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.73725490196078436</v>
+      </c>
+      <c r="AA3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.75294117647058822</v>
+      </c>
+      <c r="AB3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.792156862745098</v>
+      </c>
+      <c r="AC3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.83529411764705885</v>
+      </c>
+      <c r="AD3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.86274509803921573</v>
+      </c>
+      <c r="AE3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.90588235294117647</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="19"/>
+      <c r="R5" s="3">
+        <f>1.020768*R2^0.471221</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="3">
+        <f t="shared" ref="S5:AE5" si="2">1.020768*S2^0.471221</f>
+        <v>0.19974216060338268</v>
+      </c>
+      <c r="T5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.36045083111300397</v>
+      </c>
+      <c r="U5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.48688879058624562</v>
+      </c>
+      <c r="V5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.53604052193122609</v>
+      </c>
+      <c r="W5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.56617623751681545</v>
+      </c>
+      <c r="X5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.62159610559607681</v>
+      </c>
+      <c r="Y5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.69561422374988136</v>
+      </c>
+      <c r="Z5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.73769419449196283</v>
+      </c>
+      <c r="AA5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.75379148411571406</v>
+      </c>
+      <c r="AB5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.79494059535855732</v>
+      </c>
+      <c r="AC5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.84323601606877319</v>
+      </c>
+      <c r="AD5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.87077885797658827</v>
+      </c>
+      <c r="AE5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.9146285510902108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
       <c r="C6">
-        <v>0.2</v>
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>28</v>
+      </c>
+      <c r="E6">
+        <v>53</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F14" si="0">COS(C6)</f>
-        <v>0.98006657784124163</v>
+        <v>65</v>
+      </c>
+      <c r="G6">
+        <v>73</v>
+      </c>
+      <c r="H6">
+        <v>89</v>
+      </c>
+      <c r="I6">
+        <v>113</v>
+      </c>
+      <c r="J6">
+        <v>128</v>
+      </c>
+      <c r="K6">
+        <v>134</v>
+      </c>
+      <c r="L6">
+        <v>150</v>
+      </c>
+      <c r="M6">
+        <v>170</v>
+      </c>
+      <c r="N6">
+        <v>182</v>
+      </c>
+      <c r="O6" s="20">
+        <v>202</v>
+      </c>
+      <c r="R6" s="4">
+        <f>R5*255</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="4">
+        <f t="shared" ref="S6:AE6" si="3">S5*255</f>
+        <v>50.934250953862581</v>
+      </c>
+      <c r="T6" s="4">
+        <f t="shared" si="3"/>
+        <v>91.914961933816016</v>
+      </c>
+      <c r="U6" s="4">
+        <f t="shared" si="3"/>
+        <v>124.15664159949263</v>
+      </c>
+      <c r="V6" s="4">
+        <f t="shared" si="3"/>
+        <v>136.69033309246265</v>
+      </c>
+      <c r="W6" s="4">
+        <f t="shared" si="3"/>
+        <v>144.37494056678793</v>
+      </c>
+      <c r="X6" s="4">
+        <f t="shared" si="3"/>
+        <v>158.50700692699959</v>
+      </c>
+      <c r="Y6" s="4">
+        <f t="shared" si="3"/>
+        <v>177.38162705621974</v>
+      </c>
+      <c r="Z6" s="4">
+        <f t="shared" si="3"/>
+        <v>188.11201959545053</v>
+      </c>
+      <c r="AA6" s="4">
+        <f t="shared" si="3"/>
+        <v>192.21682844950709</v>
+      </c>
+      <c r="AB6" s="4">
+        <f t="shared" si="3"/>
+        <v>202.70985181643212</v>
+      </c>
+      <c r="AC6" s="4">
+        <f t="shared" si="3"/>
+        <v>215.02518409753716</v>
+      </c>
+      <c r="AD6" s="4">
+        <f t="shared" si="3"/>
+        <v>222.04860878403002</v>
+      </c>
+      <c r="AE6" s="4">
+        <f t="shared" si="3"/>
+        <v>233.23028052800376</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>0.3</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>0.95533648912560598</v>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="16">
+        <v>127</v>
+      </c>
+      <c r="C7" s="16">
+        <v>127</v>
+      </c>
+      <c r="D7" s="16">
+        <v>130</v>
+      </c>
+      <c r="E7" s="16">
+        <v>121</v>
+      </c>
+      <c r="F7" s="16">
+        <v>168</v>
+      </c>
+      <c r="G7" s="16">
+        <v>116</v>
+      </c>
+      <c r="H7" s="16">
+        <v>126</v>
+      </c>
+      <c r="I7" s="16">
+        <v>72</v>
+      </c>
+      <c r="J7" s="16">
+        <v>128</v>
+      </c>
+      <c r="K7" s="16">
+        <v>118</v>
+      </c>
+      <c r="L7" s="16">
+        <v>58</v>
+      </c>
+      <c r="M7" s="16">
+        <v>90</v>
+      </c>
+      <c r="N7" s="16">
+        <v>179</v>
+      </c>
+      <c r="O7" s="21">
+        <v>102</v>
+      </c>
+      <c r="R7" s="4">
+        <f>R6-B2</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="4">
+        <f t="shared" ref="S7:AE7" si="4">S6-C2</f>
+        <v>0.9342509538625805</v>
+      </c>
+      <c r="T7" s="4">
+        <f t="shared" si="4"/>
+        <v>-1.0850380661839836</v>
+      </c>
+      <c r="U7" s="4">
+        <f t="shared" si="4"/>
+        <v>-0.84335840050736977</v>
+      </c>
+      <c r="V7" s="4">
+        <f t="shared" si="4"/>
+        <v>-1.3096669075373484</v>
+      </c>
+      <c r="W7" s="4">
+        <f t="shared" si="4"/>
+        <v>-1.6250594332120727</v>
+      </c>
+      <c r="X7" s="4">
+        <f t="shared" si="4"/>
+        <v>-1.492993073000406</v>
+      </c>
+      <c r="Y7" s="4">
+        <f t="shared" si="4"/>
+        <v>-0.61837294378025831</v>
+      </c>
+      <c r="Z7" s="4">
+        <f t="shared" si="4"/>
+        <v>0.11201959545053342</v>
+      </c>
+      <c r="AA7" s="4">
+        <f t="shared" si="4"/>
+        <v>0.21682844950709068</v>
+      </c>
+      <c r="AB7" s="4">
+        <f t="shared" si="4"/>
+        <v>0.70985181643212059</v>
+      </c>
+      <c r="AC7" s="4">
+        <f t="shared" si="4"/>
+        <v>2.0251840975371636</v>
+      </c>
+      <c r="AD7" s="4">
+        <f t="shared" si="4"/>
+        <v>2.0486087840300229</v>
+      </c>
+      <c r="AE7" s="4">
+        <f t="shared" si="4"/>
+        <v>2.2302805280037603</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>0.4</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>0.9210609940028851</v>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <f>B6/255</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
+        <f>C6/255</f>
+        <v>3.1372549019607843E-2</v>
+      </c>
+      <c r="D13" s="3">
+        <f>D6/255</f>
+        <v>0.10980392156862745</v>
+      </c>
+      <c r="E13" s="3">
+        <f>E6/255</f>
+        <v>0.20784313725490197</v>
+      </c>
+      <c r="F13" s="3">
+        <f>F6/255</f>
+        <v>0.25490196078431371</v>
+      </c>
+      <c r="G13" s="3">
+        <f>G6/255</f>
+        <v>0.28627450980392155</v>
+      </c>
+      <c r="H13" s="3">
+        <f>H6/255</f>
+        <v>0.34901960784313724</v>
+      </c>
+      <c r="I13" s="3">
+        <f>I6/255</f>
+        <v>0.44313725490196076</v>
+      </c>
+      <c r="J13" s="3">
+        <f>J6/255</f>
+        <v>0.50196078431372548</v>
+      </c>
+      <c r="K13" s="3">
+        <f>K6/255</f>
+        <v>0.52549019607843139</v>
+      </c>
+      <c r="L13" s="3">
+        <f>L6/255</f>
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="M13" s="3">
+        <f>M6/255</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N13" s="3">
+        <f>N6/255</f>
+        <v>0.71372549019607845</v>
+      </c>
+      <c r="O13" s="3">
+        <f>O6/255</f>
+        <v>0.792156862745098</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>0.5</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>0.87758256189037276</v>
-      </c>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <v>0.6</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>0.82533561490967833</v>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <f>(B13)^0.4</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" ref="C15:O15" si="5">(C13)^0.4</f>
+        <v>0.25039169646421544</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="5"/>
+        <v>0.41328261840213837</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="5"/>
+        <v>0.53345068319099676</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="5"/>
+        <v>0.57882765232100541</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="5"/>
+        <v>0.60633560558880195</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" si="5"/>
+        <v>0.65635671158206876</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="5"/>
+        <v>0.72212986302440352</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="5"/>
+        <v>0.75904568489490887</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="5"/>
+        <v>0.77308250848003324</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" si="5"/>
+        <v>0.80876142993598876</v>
+      </c>
+      <c r="M15" s="3">
+        <f t="shared" si="5"/>
+        <v>0.85028300041719385</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" si="5"/>
+        <v>0.87380089060550592</v>
+      </c>
+      <c r="O15" s="3">
+        <f t="shared" si="5"/>
+        <v>0.91101279291599613</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>0.7</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>0.7648421872844885</v>
-      </c>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <v>0.8</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0.69670670934716539</v>
-      </c>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>0.9</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>0.62160996827066439</v>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <f>B15*255</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" ref="C18:O18" si="6">C15*255</f>
+        <v>63.84988259837494</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="6"/>
+        <v>105.38706769254529</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="6"/>
+        <v>136.02992421370416</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="6"/>
+        <v>147.60105134185639</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="6"/>
+        <v>154.61557942514449</v>
+      </c>
+      <c r="H18" s="4">
+        <f t="shared" si="6"/>
+        <v>167.37096145342753</v>
+      </c>
+      <c r="I18" s="4">
+        <f t="shared" si="6"/>
+        <v>184.14311507122289</v>
+      </c>
+      <c r="J18" s="4">
+        <f t="shared" si="6"/>
+        <v>193.55664964820176</v>
+      </c>
+      <c r="K18" s="4">
+        <f t="shared" si="6"/>
+        <v>197.13603966240848</v>
+      </c>
+      <c r="L18" s="4">
+        <f t="shared" si="6"/>
+        <v>206.23416463367712</v>
+      </c>
+      <c r="M18" s="4">
+        <f t="shared" si="6"/>
+        <v>216.82216510638443</v>
+      </c>
+      <c r="N18" s="4">
+        <f t="shared" si="6"/>
+        <v>222.81922710440401</v>
+      </c>
+      <c r="O18" s="4">
+        <f t="shared" si="6"/>
+        <v>232.30826219357903</v>
       </c>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>0.54030230586813977</v>
-      </c>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <f>B2-B18</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" ref="C19:O19" si="7">C2-C18</f>
+        <v>-13.84988259837494</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" si="7"/>
+        <v>-12.387067692545287</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="7"/>
+        <v>-11.029924213704163</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" si="7"/>
+        <v>-9.6010513418563903</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="7"/>
+        <v>-8.6155794251444888</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="7"/>
+        <v>-7.3709614534275261</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" si="7"/>
+        <v>-6.1431150712228941</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="7"/>
+        <v>-5.5566496482017556</v>
+      </c>
+      <c r="K19" s="4">
+        <f t="shared" si="7"/>
+        <v>-5.1360396624084785</v>
+      </c>
+      <c r="L19" s="4">
+        <f t="shared" si="7"/>
+        <v>-4.2341646336771248</v>
+      </c>
+      <c r="M19" s="4">
+        <f t="shared" si="7"/>
+        <v>-3.822165106384432</v>
+      </c>
+      <c r="N19" s="4">
+        <f t="shared" si="7"/>
+        <v>-2.8192271044040069</v>
+      </c>
+      <c r="O19" s="4">
+        <f t="shared" si="7"/>
+        <v>-1.3082621935790257</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>